<commit_message>
Added passed_test file to test last timing changes
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/word_lists/practice_word_freq_list.xlsx
+++ b/experiment/RUN_ME/stimuli/word_lists/practice_word_freq_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\word_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D14B51-F320-46AF-ACE9-BF7DB167C252}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9770C2BF-948E-47DD-A61E-A9342B6127ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,18 +195,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -239,41 +233,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -323,16 +346,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0" tableBorderDxfId="5">
   <autoFilter ref="A1:D21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
     <sortCondition ref="A1:A31"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="natural" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="natural_freq"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="artificial"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="artificail_freq"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="natural" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="natural_freq" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="artificial" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="artificail_freq" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -604,7 +627,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -617,221 +640,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="12" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
@@ -847,8 +874,8 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -882,7 +909,7 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="5"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>